<commit_message>
finished 1-6 but was having trouble with bonus
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b6a4b543f6f8d169/Documents/DA11/Excel/lookups-exercise-jmcapps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="8_{19ED61FC-0AAB-4DAC-83F6-00D6AC42053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4FADF87-6E8A-4F85-84D0-9B52B04AF12E}"/>
+  <xr:revisionPtr revIDLastSave="167" documentId="8_{19ED61FC-0AAB-4DAC-83F6-00D6AC42053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{221A0391-AE73-4349-B9F7-29918E36C35A}"/>
   <bookViews>
-    <workbookView xWindow="5328" yWindow="96" windowWidth="17280" windowHeight="11352" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9720" yWindow="96" windowWidth="12888" windowHeight="11352" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -915,8 +915,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Administrative</a:t>
+              <a:t>Budget</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs Actual</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1836,16 +1841,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>899160</xdr:colOff>
       <xdr:row>86</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2176,8 +2181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5398,15 +5403,15 @@
         <v>24</v>
       </c>
       <c r="B65">
-        <f>_xlfn.XLOOKUP(A65,A2:A52,D2:D52)</f>
+        <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$D$2:$D$52)</f>
         <v>36209.630000000005</v>
       </c>
       <c r="C65">
-        <f>_xlfn.XLOOKUP(A65,A2:A52,I2:I52)</f>
+        <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$I$2:$I$52)</f>
         <v>27292.159999999974</v>
       </c>
       <c r="D65">
-        <f>_xlfn.XLOOKUP(A65,A2:A52,N2:N52)</f>
+        <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$N$2:$N$52)</f>
         <v>9181.0800000000163</v>
       </c>
     </row>
@@ -5415,15 +5420,15 @@
         <v>25</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B70" si="9">_xlfn.XLOOKUP(A66,A3:A53,D3:D53)</f>
+        <f t="shared" ref="B66:B70" si="9">_xlfn.XLOOKUP(A66,$A$2:$A$52,$D$2:$D$52)</f>
         <v>0</v>
       </c>
       <c r="C66">
-        <f t="shared" ref="C66:C70" si="10">_xlfn.XLOOKUP(A66,A3:A53,I3:I53)</f>
+        <f t="shared" ref="C66:C70" si="10">_xlfn.XLOOKUP(A66,$A$2:$A$52,$I$2:$I$52)</f>
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D70" si="11">_xlfn.XLOOKUP(A66,A3:A53,N3:N53)</f>
+        <f t="shared" ref="D66:D70" si="11">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52)</f>
         <v>311228.08999999997</v>
       </c>
     </row>

</xml_diff>